<commit_message>
updated gant chart a little, update with your stuff
</commit_message>
<xml_diff>
--- a/SP4 Proposal and FrameWork/Charts + Diagrams + Reports/SP4 Gantt Project Planner v1.xlsx
+++ b/SP4 Proposal and FrameWork/Charts + Diagrams + Reports/SP4 Gantt Project Planner v1.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Project Planner</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>Buying During Game -- WQ</t>
+  </si>
+  <si>
+    <t>Highscore Class - R</t>
+  </si>
+  <si>
+    <t>Modelling - WQ</t>
   </si>
 </sst>
 </file>
@@ -329,7 +335,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +380,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,7 +464,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -518,6 +536,15 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -530,7 +557,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="58">
     <dxf>
       <fill>
         <patternFill>
@@ -671,6 +698,571 @@
         </top>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1094,10 +1686,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BQ35"/>
+  <dimension ref="B2:BQ38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9:Y28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1482,6 +2074,7 @@
       <c r="G15" s="17">
         <v>1</v>
       </c>
+      <c r="O15" s="12"/>
     </row>
     <row r="16" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="21" t="s">
@@ -1562,6 +2155,8 @@
       <c r="G19" s="17">
         <v>1</v>
       </c>
+      <c r="P19" s="12"/>
+      <c r="R19" s="24"/>
       <c r="BO19" s="22"/>
     </row>
     <row r="20" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1598,7 +2193,7 @@
         <v>8</v>
       </c>
       <c r="F21" s="16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21" s="17">
         <v>1</v>
@@ -1624,75 +2219,68 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="1">
+        <v>15</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1">
+        <v>15</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1</v>
+      </c>
+      <c r="X23" s="26"/>
+    </row>
+    <row r="24" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="1">
+        <v>12</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>12</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7">
+        <v>1</v>
+      </c>
+      <c r="X24" s="25"/>
+    </row>
     <row r="25" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="20" t="s">
+      <c r="X25" s="25"/>
+    </row>
+    <row r="26" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X26" s="25"/>
+    </row>
+    <row r="27" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="2" t="s">
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C26" s="16">
-        <v>0</v>
-      </c>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16">
-        <v>0</v>
-      </c>
-      <c r="F26" s="16">
-        <v>0</v>
-      </c>
-      <c r="G26" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="16">
-        <v>0</v>
-      </c>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16">
-        <v>0</v>
-      </c>
-      <c r="F27" s="16">
-        <v>0</v>
-      </c>
-      <c r="G27" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="16">
-        <v>0</v>
-      </c>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16">
-        <v>0</v>
-      </c>
-      <c r="F28" s="16">
-        <v>0</v>
-      </c>
-      <c r="G28" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="21" t="s">
-        <v>25</v>
       </c>
       <c r="C29" s="16">
         <v>0</v>
@@ -1709,8 +2297,8 @@
       </c>
     </row>
     <row r="30" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="21" t="s">
-        <v>26</v>
+      <c r="B30" s="15" t="s">
+        <v>23</v>
       </c>
       <c r="C30" s="16">
         <v>0</v>
@@ -1728,7 +2316,7 @@
     </row>
     <row r="31" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C31" s="16">
         <v>0</v>
@@ -1746,7 +2334,7 @@
     </row>
     <row r="32" spans="2:67" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C32" s="16">
         <v>0</v>
@@ -1762,9 +2350,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="15" t="s">
-        <v>22</v>
+    <row r="33" spans="2:19" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="C33" s="16">
         <v>0</v>
@@ -1780,16 +2368,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:19" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="21" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C34" s="16">
         <v>0</v>
       </c>
       <c r="D34" s="16"/>
       <c r="E34" s="16">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F34" s="16">
         <v>0</v>
@@ -1798,12 +2386,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="2:19" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="16">
+        <v>0</v>
+      </c>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16">
+        <v>0</v>
+      </c>
+      <c r="F35" s="16">
+        <v>0</v>
+      </c>
+      <c r="G35" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="16">
+        <v>0</v>
+      </c>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16">
+        <v>0</v>
+      </c>
+      <c r="F36" s="16">
+        <v>0</v>
+      </c>
+      <c r="G36" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="16">
+        <v>0</v>
+      </c>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16">
+        <v>11</v>
+      </c>
+      <c r="F37" s="16">
+        <v>1</v>
+      </c>
+      <c r="G37" s="17">
+        <v>1</v>
+      </c>
+      <c r="R37" s="26"/>
+      <c r="S37" s="12"/>
+    </row>
+    <row r="38" spans="2:19" ht="18.95" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:BP18 I20:BP35 I19:AC19">
+  <conditionalFormatting sqref="I9:BP14 I20:BP22 I19:O19 I27:BP36 I23:W26 Y23:BP26 I38:BP38 I37:Q37 T37:BP37 I16:BP18 I15:N15 P15:BP15 Q19:AC19">
     <cfRule type="expression" dxfId="17" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1829,7 +2473,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36:BP36">
+  <conditionalFormatting sqref="B39:BP39">
     <cfRule type="expression" dxfId="9" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>